<commit_message>
add download all ratios
</commit_message>
<xml_diff>
--- a/data/staff_table.xlsx
+++ b/data/staff_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aekrumm/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xilinchen/Documents/Repo/staff_projection/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895B280D-D448-3341-BDA2-C34BA4B7AB10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D3C4AA-20D2-FC44-B73D-93C0105CDFAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6260" yWindow="2920" windowWidth="27240" windowHeight="16440" xr2:uid="{18556180-8EE1-D541-B86E-C93BDDD14B2F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
   <si>
     <t>team_type</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Respiratory Thrapist</t>
-  </si>
-  <si>
-    <t>Pharn</t>
   </si>
   <si>
     <t>Fellow / Non-CC Attending</t>
@@ -436,7 +433,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,10 +446,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -502,7 +499,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -558,7 +555,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>15</v>
@@ -572,7 +569,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>12</v>
@@ -586,7 +583,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>12</v>
@@ -600,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -611,7 +608,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -625,7 +622,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -639,7 +636,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -653,10 +650,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -667,7 +664,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -681,7 +678,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -695,7 +692,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -709,10 +706,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20">
         <v>30</v>
@@ -723,10 +720,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21">
         <v>30</v>

</xml_diff>